<commit_message>
bhumeswor valuation given and indrayani roof estimate only to ram mani and hakim
</commit_message>
<xml_diff>
--- a/ofc/estimates/Finalized valuations/indrayani mandir/full estimate - Copy.xlsx
+++ b/ofc/estimates/Finalized valuations/indrayani mandir/full estimate - Copy.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="quotation" sheetId="4" r:id="rId2"/>
+    <sheet name="quotation (2)" sheetId="5" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
     <definedName name="description_124" localSheetId="0">#REF!</definedName>
     <definedName name="description_124" localSheetId="1">#REF!</definedName>
+    <definedName name="description_124" localSheetId="2">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
     <definedName name="description_247">[1]Abstract!$B$22</definedName>
     <definedName name="description_261">[2]Abstract!$B$33</definedName>
@@ -28,6 +30,7 @@
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">final!$A$1:$K$272</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">quotation!$A$6:$K$246</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'quotation (2)'!$A$6:$K$52</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">final!$1:$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="132">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -450,6 +453,9 @@
   <si>
     <t xml:space="preserve">F.Y.: 2081/2082      </t>
   </si>
+  <si>
+    <t>20 gauge Brass plate making and fixing on roof</t>
+  </si>
 </sst>
 </file>
 
@@ -826,27 +832,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,11 +850,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1342,113 +1348,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
     </row>
     <row r="8" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -7277,11 +7283,11 @@
       <c r="B267" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C267" s="76">
+      <c r="C267" s="82">
         <f>J265</f>
         <v>1886794.504041455</v>
       </c>
-      <c r="D267" s="77"/>
+      <c r="D267" s="83"/>
       <c r="E267" s="33">
         <v>100</v>
       </c>
@@ -7296,21 +7302,21 @@
       <c r="B268" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C268" s="80">
+      <c r="C268" s="85">
         <v>2250000</v>
       </c>
-      <c r="D268" s="81"/>
+      <c r="D268" s="86"/>
       <c r="E268" s="33"/>
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B269" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C269" s="80">
+      <c r="C269" s="85">
         <f>C268-C271-C272</f>
         <v>2137500</v>
       </c>
-      <c r="D269" s="81"/>
+      <c r="D269" s="86"/>
       <c r="E269" s="33">
         <f>C269/C267*100</f>
         <v>113.28737684053785</v>
@@ -7320,11 +7326,11 @@
       <c r="B270" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C270" s="82">
+      <c r="C270" s="87">
         <f>C267-C269</f>
         <v>-250705.49595854501</v>
       </c>
-      <c r="D270" s="82"/>
+      <c r="D270" s="87"/>
       <c r="E270" s="33">
         <f>100-E269</f>
         <v>-13.287376840537846</v>
@@ -7334,11 +7340,11 @@
       <c r="B271" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C271" s="76">
+      <c r="C271" s="82">
         <f>C268*0.03</f>
         <v>67500</v>
       </c>
-      <c r="D271" s="77"/>
+      <c r="D271" s="83"/>
       <c r="E271" s="33">
         <v>3</v>
       </c>
@@ -7347,24 +7353,17 @@
       <c r="B272" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="C272" s="76">
+      <c r="C272" s="82">
         <f>C268*0.02</f>
         <v>45000</v>
       </c>
-      <c r="D272" s="77"/>
+      <c r="D272" s="83"/>
       <c r="E272" s="33">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C271:D271"/>
     <mergeCell ref="C272:D272"/>
     <mergeCell ref="A7:F7"/>
@@ -7373,6 +7372,13 @@
     <mergeCell ref="C268:D268"/>
     <mergeCell ref="C269:D269"/>
     <mergeCell ref="C270:D270"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7390,8 +7396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView topLeftCell="A220" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G221" sqref="G221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7411,113 +7417,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="84" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
     </row>
     <row r="8" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -12815,12 +12821,12 @@
       <c r="B239" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C239" s="82">
+      <c r="C239" s="87">
         <f>J237</f>
         <v>2108070.4791162037</v>
       </c>
-      <c r="D239" s="82"/>
-      <c r="E239" s="82"/>
+      <c r="D239" s="87"/>
+      <c r="E239" s="87"/>
       <c r="F239" s="65"/>
       <c r="G239" s="66"/>
       <c r="H239" s="65"/>
@@ -12832,21 +12838,21 @@
       <c r="B240" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C240" s="88">
+      <c r="C240" s="89">
         <v>2250000</v>
       </c>
-      <c r="D240" s="88"/>
+      <c r="D240" s="89"/>
       <c r="E240" s="33"/>
     </row>
     <row r="241" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B241" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C241" s="88">
+      <c r="C241" s="89">
         <f>C240-C243-C244</f>
         <v>2137500</v>
       </c>
-      <c r="D241" s="88"/>
+      <c r="D241" s="89"/>
       <c r="E241" s="33">
         <f>C241/C239*100</f>
         <v>101.39604065306843</v>
@@ -12856,11 +12862,11 @@
       <c r="B242" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C242" s="82">
+      <c r="C242" s="87">
         <f>C239-C241</f>
         <v>-29429.520883796271</v>
       </c>
-      <c r="D242" s="82"/>
+      <c r="D242" s="87"/>
       <c r="E242" s="33">
         <f>100-E241</f>
         <v>-1.3960406530684253</v>
@@ -12870,11 +12876,11 @@
       <c r="B243" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C243" s="82">
+      <c r="C243" s="87">
         <f>C240*0.03</f>
         <v>67500</v>
       </c>
-      <c r="D243" s="82"/>
+      <c r="D243" s="87"/>
       <c r="E243" s="33">
         <v>3</v>
       </c>
@@ -12883,11 +12889,11 @@
       <c r="B244" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="C244" s="82">
+      <c r="C244" s="87">
         <f>C240*0.02</f>
         <v>45000</v>
       </c>
-      <c r="D244" s="82"/>
+      <c r="D244" s="87"/>
       <c r="E244" s="33">
         <v>2</v>
       </c>
@@ -12896,36 +12902,26 @@
       <c r="B245" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="C245" s="89">
+      <c r="C245" s="88">
         <f>C239*0.13</f>
         <v>274049.16228510649</v>
       </c>
-      <c r="D245" s="89"/>
-      <c r="E245" s="89"/>
+      <c r="D245" s="88"/>
+      <c r="E245" s="88"/>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="C246" s="89">
+      <c r="C246" s="88">
         <f>C239+C245</f>
         <v>2382119.6414013105</v>
       </c>
-      <c r="D246" s="89"/>
-      <c r="E246" s="89"/>
+      <c r="D246" s="88"/>
+      <c r="E246" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C243:D243"/>
-    <mergeCell ref="C244:D244"/>
-    <mergeCell ref="C245:E245"/>
-    <mergeCell ref="C246:E246"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C240:D240"/>
-    <mergeCell ref="C241:D241"/>
-    <mergeCell ref="C242:D242"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -12933,6 +12929,1064 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C240:D240"/>
+    <mergeCell ref="C241:D241"/>
+    <mergeCell ref="C242:D242"/>
+    <mergeCell ref="C243:D243"/>
+    <mergeCell ref="C244:D244"/>
+    <mergeCell ref="C245:E245"/>
+    <mergeCell ref="C246:E246"/>
+    <mergeCell ref="C239:E239"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="71" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="71" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="71" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="71" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+    </row>
+    <row r="8" spans="1:19" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>32</v>
+      </c>
+      <c r="B9" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="16"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15">
+        <f>((15.667+16.25)/2)/3.281</f>
+        <v>4.8639134410240779</v>
+      </c>
+      <c r="E10" s="16">
+        <f>((10.75)/3.281)</f>
+        <v>3.2764401097226452</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17">
+        <f t="shared" ref="G10" si="0">PRODUCT(C10:F10)</f>
+        <v>31.872642176780758</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="16"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+    </row>
+    <row r="11" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="27">
+        <f>0*SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="28">
+        <f>(325188.75/100)</f>
+        <v>3251.8874999999998</v>
+      </c>
+      <c r="J11" s="29">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="30"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="39">
+        <f>0.13*G11*((221748.75)/100)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>33</v>
+      </c>
+      <c r="B14" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="30"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="14">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="D15" s="15">
+        <f>D10</f>
+        <v>4.8639134410240779</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17">
+        <f>PRODUCT(C15:F15)</f>
+        <v>19.455653764096311</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="16"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="27">
+        <f>0*SUM(G15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="28">
+        <v>1842.85</v>
+      </c>
+      <c r="J16" s="29">
+        <f>G16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="30"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="39">
+        <f>0.13*G16*((164000)/100)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>34</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="26">
+        <v>4</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17">
+        <f t="shared" ref="G20" si="1">PRODUCT(C20:F20)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="27">
+        <f>0*SUM(G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="28">
+        <v>279</v>
+      </c>
+      <c r="J21" s="29">
+        <f>G21*I21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="39">
+        <f>0.13*J21</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="30"/>
+    </row>
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="30"/>
+    </row>
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>1</v>
+      </c>
+      <c r="B24" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="16"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="14">
+        <v>2</v>
+      </c>
+      <c r="D25" s="15">
+        <f>(((15.667+16.25)/2)/3.281)+0.2</f>
+        <v>5.063913441024078</v>
+      </c>
+      <c r="E25" s="16">
+        <f>((10.75)/3.281)</f>
+        <v>3.2764401097226452</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17">
+        <f t="shared" ref="G25" si="2">PRODUCT(C25:F25)</f>
+        <v>33.183218220669815</v>
+      </c>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="16"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="27">
+        <f>SUM(G25:G25)</f>
+        <v>33.183218220669815</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="28">
+        <v>14913.64</v>
+      </c>
+      <c r="J26" s="29">
+        <f>G26*I26</f>
+        <v>494882.57058451016</v>
+      </c>
+      <c r="K26" s="30"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="30"/>
+    </row>
+    <row r="28" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>2</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="30"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="14">
+        <v>2</v>
+      </c>
+      <c r="D29" s="16">
+        <f>((10.75)/3.281)</f>
+        <v>3.2764401097226452</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17">
+        <f t="shared" ref="G29" si="3">PRODUCT(C29:F29)</f>
+        <v>6.5528802194452904</v>
+      </c>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="16"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="27">
+        <f>SUM(G29:G29)</f>
+        <v>6.5528802194452904</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="28">
+        <f>2563.07</f>
+        <v>2563.0700000000002</v>
+      </c>
+      <c r="J30" s="29">
+        <f>G30*I30</f>
+        <v>16795.490704053642</v>
+      </c>
+      <c r="K30" s="30"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="30"/>
+    </row>
+    <row r="32" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="25">
+        <v>3</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="30"/>
+    </row>
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="14">
+        <v>4</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17">
+        <f t="shared" ref="G33" si="4">PRODUCT(C33:F33)</f>
+        <v>4</v>
+      </c>
+      <c r="H33" s="18"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="16"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+    </row>
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="27">
+        <f>SUM(G33:G33)</f>
+        <v>4</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="28">
+        <f>6970.73</f>
+        <v>6970.73</v>
+      </c>
+      <c r="J34" s="29">
+        <f>G34*I34</f>
+        <v>27882.92</v>
+      </c>
+      <c r="K34" s="30"/>
+    </row>
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="30"/>
+    </row>
+    <row r="36" spans="1:19" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
+        <v>4</v>
+      </c>
+      <c r="B36" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="32">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="D36" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33">
+        <f>PRODUCT(C36:F36)</f>
+        <v>10.5</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="34"/>
+    </row>
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="26"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="27">
+        <f>SUM(G36:G36)</f>
+        <v>10.5</v>
+      </c>
+      <c r="H37" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37" s="27">
+        <f>4289.73</f>
+        <v>4289.7299999999996</v>
+      </c>
+      <c r="J37" s="29">
+        <f>G36*I37</f>
+        <v>45042.164999999994</v>
+      </c>
+      <c r="K37" s="30"/>
+    </row>
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="30"/>
+    </row>
+    <row r="39" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>5</v>
+      </c>
+      <c r="B39" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="32">
+        <v>1</v>
+      </c>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="37">
+        <f>PRODUCT(C39:F39)</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="I39" s="37">
+        <v>150000</v>
+      </c>
+      <c r="J39" s="39">
+        <f>G39*I39</f>
+        <v>150000</v>
+      </c>
+      <c r="K39" s="34"/>
+    </row>
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="30"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>6</v>
+      </c>
+      <c r="B41" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="14">
+        <v>1</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="37">
+        <f t="shared" ref="G41" si="5">PRODUCT(C41:F41)</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I41" s="19">
+        <v>1000</v>
+      </c>
+      <c r="J41" s="37">
+        <f>G41*I41</f>
+        <v>1000</v>
+      </c>
+      <c r="K41" s="16"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+    </row>
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="16"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="25"/>
+      <c r="B43" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="63"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20">
+        <f>SUM(J9:J41)</f>
+        <v>735603.14628856385</v>
+      </c>
+      <c r="K43" s="30"/>
+    </row>
+    <row r="45" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="87">
+        <f>J43</f>
+        <v>735603.14628856385</v>
+      </c>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="68"/>
+      <c r="K45" s="69"/>
+    </row>
+    <row r="46" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="89">
+        <v>2250000</v>
+      </c>
+      <c r="D46" s="89"/>
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="89">
+        <f>C46-C49-C50</f>
+        <v>2137500</v>
+      </c>
+      <c r="D47" s="89"/>
+      <c r="E47" s="33">
+        <f>C47/C45*100</f>
+        <v>290.57787623457193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="87">
+        <f>C45-C47</f>
+        <v>-1401896.853711436</v>
+      </c>
+      <c r="D48" s="87"/>
+      <c r="E48" s="33">
+        <f>100-E47</f>
+        <v>-190.57787623457193</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="87">
+        <f>C46*0.03</f>
+        <v>67500</v>
+      </c>
+      <c r="D49" s="87"/>
+      <c r="E49" s="33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="87">
+        <f>C46*0.02</f>
+        <v>45000</v>
+      </c>
+      <c r="D50" s="87"/>
+      <c r="E50" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="88">
+        <f>C45*0.13</f>
+        <v>95628.409017513302</v>
+      </c>
+      <c r="D51" s="88"/>
+      <c r="E51" s="88"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="88">
+        <f>C45+C51</f>
+        <v>831231.55530607712</v>
+      </c>
+      <c r="D52" s="88"/>
+      <c r="E52" s="88"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
small edit in indrayani mandir roof estimate
</commit_message>
<xml_diff>
--- a/ofc/estimates/Finalized valuations/indrayani mandir/full estimate - Copy.xlsx
+++ b/ofc/estimates/Finalized valuations/indrayani mandir/full estimate - Copy.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="quotation" sheetId="4" r:id="rId2"/>
     <sheet name="quotation (2)" sheetId="5" r:id="rId3"/>
+    <sheet name="with plastic felt" sheetId="6" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
     <definedName name="description_124" localSheetId="0">#REF!</definedName>
     <definedName name="description_124" localSheetId="1">#REF!</definedName>
     <definedName name="description_124" localSheetId="2">#REF!</definedName>
+    <definedName name="description_124" localSheetId="3">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
     <definedName name="description_247">[1]Abstract!$B$22</definedName>
     <definedName name="description_261">[2]Abstract!$B$33</definedName>
@@ -31,6 +33,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">final!$A$1:$K$272</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">quotation!$A$6:$K$246</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'quotation (2)'!$A$6:$K$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'with plastic felt'!$A$6:$K$56</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">final!$1:$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="132">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -832,11 +835,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -850,27 +869,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1348,113 +1351,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -7283,11 +7286,11 @@
       <c r="B267" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C267" s="82">
+      <c r="C267" s="76">
         <f>J265</f>
         <v>1886794.504041455</v>
       </c>
-      <c r="D267" s="83"/>
+      <c r="D267" s="77"/>
       <c r="E267" s="33">
         <v>100</v>
       </c>
@@ -7302,21 +7305,21 @@
       <c r="B268" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C268" s="85">
+      <c r="C268" s="80">
         <v>2250000</v>
       </c>
-      <c r="D268" s="86"/>
+      <c r="D268" s="81"/>
       <c r="E268" s="33"/>
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B269" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C269" s="85">
+      <c r="C269" s="80">
         <f>C268-C271-C272</f>
         <v>2137500</v>
       </c>
-      <c r="D269" s="86"/>
+      <c r="D269" s="81"/>
       <c r="E269" s="33">
         <f>C269/C267*100</f>
         <v>113.28737684053785</v>
@@ -7326,11 +7329,11 @@
       <c r="B270" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C270" s="87">
+      <c r="C270" s="82">
         <f>C267-C269</f>
         <v>-250705.49595854501</v>
       </c>
-      <c r="D270" s="87"/>
+      <c r="D270" s="82"/>
       <c r="E270" s="33">
         <f>100-E269</f>
         <v>-13.287376840537846</v>
@@ -7340,11 +7343,11 @@
       <c r="B271" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C271" s="82">
+      <c r="C271" s="76">
         <f>C268*0.03</f>
         <v>67500</v>
       </c>
-      <c r="D271" s="83"/>
+      <c r="D271" s="77"/>
       <c r="E271" s="33">
         <v>3</v>
       </c>
@@ -7353,17 +7356,24 @@
       <c r="B272" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="C272" s="82">
+      <c r="C272" s="76">
         <f>C268*0.02</f>
         <v>45000</v>
       </c>
-      <c r="D272" s="83"/>
+      <c r="D272" s="77"/>
       <c r="E272" s="33">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C271:D271"/>
     <mergeCell ref="C272:D272"/>
     <mergeCell ref="A7:F7"/>
@@ -7372,13 +7382,6 @@
     <mergeCell ref="C268:D268"/>
     <mergeCell ref="C269:D269"/>
     <mergeCell ref="C270:D270"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7417,113 +7420,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -12821,12 +12824,12 @@
       <c r="B239" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C239" s="87">
+      <c r="C239" s="82">
         <f>J237</f>
         <v>2108070.4791162037</v>
       </c>
-      <c r="D239" s="87"/>
-      <c r="E239" s="87"/>
+      <c r="D239" s="82"/>
+      <c r="E239" s="82"/>
       <c r="F239" s="65"/>
       <c r="G239" s="66"/>
       <c r="H239" s="65"/>
@@ -12838,21 +12841,21 @@
       <c r="B240" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C240" s="89">
+      <c r="C240" s="88">
         <v>2250000</v>
       </c>
-      <c r="D240" s="89"/>
+      <c r="D240" s="88"/>
       <c r="E240" s="33"/>
     </row>
     <row r="241" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B241" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C241" s="89">
+      <c r="C241" s="88">
         <f>C240-C243-C244</f>
         <v>2137500</v>
       </c>
-      <c r="D241" s="89"/>
+      <c r="D241" s="88"/>
       <c r="E241" s="33">
         <f>C241/C239*100</f>
         <v>101.39604065306843</v>
@@ -12862,11 +12865,11 @@
       <c r="B242" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C242" s="87">
+      <c r="C242" s="82">
         <f>C239-C241</f>
         <v>-29429.520883796271</v>
       </c>
-      <c r="D242" s="87"/>
+      <c r="D242" s="82"/>
       <c r="E242" s="33">
         <f>100-E241</f>
         <v>-1.3960406530684253</v>
@@ -12876,11 +12879,11 @@
       <c r="B243" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C243" s="87">
+      <c r="C243" s="82">
         <f>C240*0.03</f>
         <v>67500</v>
       </c>
-      <c r="D243" s="87"/>
+      <c r="D243" s="82"/>
       <c r="E243" s="33">
         <v>3</v>
       </c>
@@ -12889,11 +12892,11 @@
       <c r="B244" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="C244" s="87">
+      <c r="C244" s="82">
         <f>C240*0.02</f>
         <v>45000</v>
       </c>
-      <c r="D244" s="87"/>
+      <c r="D244" s="82"/>
       <c r="E244" s="33">
         <v>2</v>
       </c>
@@ -12902,26 +12905,36 @@
       <c r="B245" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="C245" s="88">
+      <c r="C245" s="89">
         <f>C239*0.13</f>
         <v>274049.16228510649</v>
       </c>
-      <c r="D245" s="88"/>
-      <c r="E245" s="88"/>
+      <c r="D245" s="89"/>
+      <c r="E245" s="89"/>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="C246" s="88">
+      <c r="C246" s="89">
         <f>C239+C245</f>
         <v>2382119.6414013105</v>
       </c>
-      <c r="D246" s="88"/>
-      <c r="E246" s="88"/>
+      <c r="D246" s="89"/>
+      <c r="E246" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C243:D243"/>
+    <mergeCell ref="C244:D244"/>
+    <mergeCell ref="C245:E245"/>
+    <mergeCell ref="C246:E246"/>
+    <mergeCell ref="C239:E239"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C240:D240"/>
+    <mergeCell ref="C241:D241"/>
+    <mergeCell ref="C242:D242"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -12929,16 +12942,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C240:D240"/>
-    <mergeCell ref="C241:D241"/>
-    <mergeCell ref="C242:D242"/>
-    <mergeCell ref="C243:D243"/>
-    <mergeCell ref="C244:D244"/>
-    <mergeCell ref="C245:E245"/>
-    <mergeCell ref="C246:E246"/>
-    <mergeCell ref="C239:E239"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12956,7 +12959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
@@ -12977,113 +12980,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:19" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -13869,12 +13872,12 @@
       <c r="B45" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C45" s="87">
+      <c r="C45" s="82">
         <f>J43</f>
         <v>735603.14628856385</v>
       </c>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
       <c r="F45" s="65"/>
       <c r="G45" s="66"/>
       <c r="H45" s="65"/>
@@ -13886,21 +13889,21 @@
       <c r="B46" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="89">
+      <c r="C46" s="88">
         <v>2250000</v>
       </c>
-      <c r="D46" s="89"/>
+      <c r="D46" s="88"/>
       <c r="E46" s="33"/>
     </row>
     <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="89">
+      <c r="C47" s="88">
         <f>C46-C49-C50</f>
         <v>2137500</v>
       </c>
-      <c r="D47" s="89"/>
+      <c r="D47" s="88"/>
       <c r="E47" s="33">
         <f>C47/C45*100</f>
         <v>290.57787623457193</v>
@@ -13910,11 +13913,11 @@
       <c r="B48" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="87">
+      <c r="C48" s="82">
         <f>C45-C47</f>
         <v>-1401896.853711436</v>
       </c>
-      <c r="D48" s="87"/>
+      <c r="D48" s="82"/>
       <c r="E48" s="33">
         <f>100-E47</f>
         <v>-190.57787623457193</v>
@@ -13924,11 +13927,11 @@
       <c r="B49" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C49" s="87">
+      <c r="C49" s="82">
         <f>C46*0.03</f>
         <v>67500</v>
       </c>
-      <c r="D49" s="87"/>
+      <c r="D49" s="82"/>
       <c r="E49" s="33">
         <v>3</v>
       </c>
@@ -13937,11 +13940,11 @@
       <c r="B50" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="87">
+      <c r="C50" s="82">
         <f>C46*0.02</f>
         <v>45000</v>
       </c>
-      <c r="D50" s="87"/>
+      <c r="D50" s="82"/>
       <c r="E50" s="33">
         <v>2</v>
       </c>
@@ -13950,36 +13953,1172 @@
       <c r="B51" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="C51" s="88">
+      <c r="C51" s="89">
         <f>C45*0.13</f>
         <v>95628.409017513302</v>
       </c>
-      <c r="D51" s="88"/>
-      <c r="E51" s="88"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="88">
+      <c r="C52" s="89">
         <f>C45+C51</f>
         <v>831231.55530607712</v>
       </c>
-      <c r="D52" s="88"/>
-      <c r="E52" s="88"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="A7:F7"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="71" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="71" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="71" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="71" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="79" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:19" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>32</v>
+      </c>
+      <c r="B9" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="16"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2</v>
+      </c>
+      <c r="D10" s="15">
+        <f>((15.667+16.25)/2)/3.281</f>
+        <v>4.8639134410240779</v>
+      </c>
+      <c r="E10" s="16">
+        <f>((10.75)/3.281)</f>
+        <v>3.2764401097226452</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17">
+        <f t="shared" ref="G10" si="0">PRODUCT(C10:F10)</f>
+        <v>31.872642176780758</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="16"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+    </row>
+    <row r="11" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="27">
+        <f>0*SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="28">
+        <f>(325188.75/100)</f>
+        <v>3251.8874999999998</v>
+      </c>
+      <c r="J11" s="29">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="30"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="39">
+        <f>0.13*G11*((221748.75)/100)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>33</v>
+      </c>
+      <c r="B14" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="30"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="14">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="D15" s="15">
+        <f>D10</f>
+        <v>4.8639134410240779</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17">
+        <f>PRODUCT(C15:F15)</f>
+        <v>19.455653764096311</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="16"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="27">
+        <f>0*SUM(G15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="28">
+        <v>1842.85</v>
+      </c>
+      <c r="J16" s="29">
+        <f>G16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="30"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="39">
+        <f>0.13*G16*((164000)/100)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>34</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="26">
+        <v>4</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17">
+        <f t="shared" ref="G20" si="1">PRODUCT(C20:F20)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="27">
+        <f>0*SUM(G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="28">
+        <v>279</v>
+      </c>
+      <c r="J21" s="29">
+        <f>G21*I21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="39">
+        <f>0.13*J21</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="30"/>
+    </row>
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="30"/>
+    </row>
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>1</v>
+      </c>
+      <c r="B24" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="16"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="14">
+        <v>2</v>
+      </c>
+      <c r="D25" s="15">
+        <f>(((15.667+16.25)/2)/3.281)+0.2</f>
+        <v>5.063913441024078</v>
+      </c>
+      <c r="E25" s="16">
+        <f>((10.75)/3.281)</f>
+        <v>3.2764401097226452</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17">
+        <f t="shared" ref="G25" si="2">PRODUCT(C25:F25)</f>
+        <v>33.183218220669815</v>
+      </c>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="16"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="27">
+        <f>SUM(G25:G25)</f>
+        <v>33.183218220669815</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="28">
+        <v>14913.64</v>
+      </c>
+      <c r="J26" s="29">
+        <f>G26*I26</f>
+        <v>494882.57058451016</v>
+      </c>
+      <c r="K26" s="30"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="30"/>
+    </row>
+    <row r="28" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>2</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="30"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="14">
+        <v>2</v>
+      </c>
+      <c r="D29" s="16">
+        <f>((10.75)/3.281)</f>
+        <v>3.2764401097226452</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17">
+        <f t="shared" ref="G29" si="3">PRODUCT(C29:F29)</f>
+        <v>6.5528802194452904</v>
+      </c>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="16"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="27">
+        <f>SUM(G29:G29)</f>
+        <v>6.5528802194452904</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="28">
+        <f>2563.07</f>
+        <v>2563.0700000000002</v>
+      </c>
+      <c r="J30" s="29">
+        <f>G30*I30</f>
+        <v>16795.490704053642</v>
+      </c>
+      <c r="K30" s="30"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="30"/>
+    </row>
+    <row r="32" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="25">
+        <v>3</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="30"/>
+    </row>
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="14">
+        <v>4</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17">
+        <f t="shared" ref="G33" si="4">PRODUCT(C33:F33)</f>
+        <v>4</v>
+      </c>
+      <c r="H33" s="18"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="16"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+    </row>
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="27">
+        <f>SUM(G33:G33)</f>
+        <v>4</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="28">
+        <f>6970.73</f>
+        <v>6970.73</v>
+      </c>
+      <c r="J34" s="29">
+        <f>G34*I34</f>
+        <v>27882.92</v>
+      </c>
+      <c r="K34" s="30"/>
+    </row>
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="30"/>
+    </row>
+    <row r="36" spans="1:19" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
+        <v>4</v>
+      </c>
+      <c r="B36" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="32">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="D36" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33">
+        <f>PRODUCT(C36:F36)</f>
+        <v>10.5</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="34"/>
+    </row>
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="26"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="27">
+        <f>SUM(G36:G36)</f>
+        <v>10.5</v>
+      </c>
+      <c r="H37" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37" s="27">
+        <f>4289.73</f>
+        <v>4289.7299999999996</v>
+      </c>
+      <c r="J37" s="29">
+        <f>G36*I37</f>
+        <v>45042.164999999994</v>
+      </c>
+      <c r="K37" s="30"/>
+    </row>
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="30"/>
+    </row>
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="25">
+        <v>5</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="26"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="30"/>
+    </row>
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="14">
+        <v>2</v>
+      </c>
+      <c r="D40" s="15">
+        <f>(((15.667+16.25)/2)/3.281)+0.2</f>
+        <v>5.063913441024078</v>
+      </c>
+      <c r="E40" s="16">
+        <f>((10.75)/3.281)</f>
+        <v>3.2764401097226452</v>
+      </c>
+      <c r="F40" s="16"/>
+      <c r="G40" s="17">
+        <f t="shared" ref="G40" si="5">PRODUCT(C40:F40)</f>
+        <v>33.183218220669815</v>
+      </c>
+      <c r="H40" s="18"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="16"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="25"/>
+      <c r="B41" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="27">
+        <f>SUM(G40:G40)</f>
+        <v>33.183218220669815</v>
+      </c>
+      <c r="H41" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" s="28">
+        <v>685.98</v>
+      </c>
+      <c r="J41" s="29">
+        <f>G41*I41</f>
+        <v>22763.024035015082</v>
+      </c>
+      <c r="K41" s="30"/>
+    </row>
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="30"/>
+    </row>
+    <row r="43" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
+        <v>6</v>
+      </c>
+      <c r="B43" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="32">
+        <v>1</v>
+      </c>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="37">
+        <f>PRODUCT(C43:F43)</f>
+        <v>1</v>
+      </c>
+      <c r="H43" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="I43" s="37">
+        <v>150000</v>
+      </c>
+      <c r="J43" s="39">
+        <f>G43*I43</f>
+        <v>150000</v>
+      </c>
+      <c r="K43" s="34"/>
+    </row>
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="30"/>
+    </row>
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
+        <v>7</v>
+      </c>
+      <c r="B45" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="14">
+        <v>1</v>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="37">
+        <f t="shared" ref="G45" si="6">PRODUCT(C45:F45)</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I45" s="19">
+        <v>1000</v>
+      </c>
+      <c r="J45" s="37">
+        <f>G45*I45</f>
+        <v>1000</v>
+      </c>
+      <c r="K45" s="16"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+    </row>
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="16"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="25"/>
+      <c r="B47" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="63"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20">
+        <f>SUM(J9:J45)</f>
+        <v>758366.17032357887</v>
+      </c>
+      <c r="K47" s="30"/>
+    </row>
+    <row r="49" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="82">
+        <f>J47</f>
+        <v>758366.17032357887</v>
+      </c>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="68"/>
+      <c r="K49" s="69"/>
+    </row>
+    <row r="50" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="88">
+        <v>2250000</v>
+      </c>
+      <c r="D50" s="88"/>
+      <c r="E50" s="33"/>
+    </row>
+    <row r="51" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="88">
+        <f>C50-C53-C54</f>
+        <v>2137500</v>
+      </c>
+      <c r="D51" s="88"/>
+      <c r="E51" s="33">
+        <f>C51/C49*100</f>
+        <v>281.8559270764905</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="82">
+        <f>C49-C51</f>
+        <v>-1379133.8296764211</v>
+      </c>
+      <c r="D52" s="82"/>
+      <c r="E52" s="33">
+        <f>100-E51</f>
+        <v>-181.8559270764905</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="82">
+        <f>C50*0.03</f>
+        <v>67500</v>
+      </c>
+      <c r="D53" s="82"/>
+      <c r="E53" s="33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="82">
+        <f>C50*0.02</f>
+        <v>45000</v>
+      </c>
+      <c r="D54" s="82"/>
+      <c r="E54" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="89">
+        <f>C49*0.13</f>
+        <v>98587.602142065254</v>
+      </c>
+      <c r="D55" s="89"/>
+      <c r="E55" s="89"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="89">
+        <f>C49+C55</f>
+        <v>856953.77246564417</v>
+      </c>
+      <c r="D56" s="89"/>
+      <c r="E56" s="89"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="A7:F7"/>
     <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>

</xml_diff>